<commit_message>
added dt plots for cartpole
</commit_message>
<xml_diff>
--- a/results/cartpole/cartpole_solved.xlsx
+++ b/results/cartpole/cartpole_solved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\antreas\rl_vfa\results\cartpole\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2313CB06-31C2-40FC-BC96-9102E14021B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D62297A-F51D-4F76-AC8C-0E8961F1ED2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="4980" windowWidth="19440" windowHeight="10824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cartpole_solved" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>n_eps</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>RF</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>SVR</t>
   </si>
 </sst>
 </file>
@@ -893,7 +899,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
@@ -1046,6 +1052,58 @@
         <v>2</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>40.130000000000003</v>
+      </c>
+      <c r="C7">
+        <v>23.62</v>
+      </c>
+      <c r="D7">
+        <v>2.36</v>
+      </c>
+      <c r="E7">
+        <v>1210.93</v>
+      </c>
+      <c r="F7">
+        <v>1937.74</v>
+      </c>
+      <c r="G7">
+        <v>193.77</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>29.48</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>0.7</v>
+      </c>
+      <c r="E8">
+        <v>682</v>
+      </c>
+      <c r="F8">
+        <v>182.32</v>
+      </c>
+      <c r="G8">
+        <v>18.23</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>

</xml_diff>